<commit_message>
Update example output to 6 factor model
</commit_message>
<xml_diff>
--- a/covid19_drdfm/data/example-output/SD/df.xlsx
+++ b/covid19_drdfm/data/example-output/SD/df.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:L133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,19 +452,54 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Prod</t>
+          <t>RPFI</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>FixAss</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>UI</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>PartR</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>UR</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cons3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Cons5</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CPIU</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>PCE</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Hosp1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -480,7 +515,28 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.2923076923076923</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -491,13 +547,34 @@
         <v>0.9868682461781157</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.7032270994259294</v>
       </c>
       <c r="D3" t="n">
+        <v>0.4737045229118747</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.2767911448733329</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
+        <v>0.9677419354838719</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9943589385115211</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.99701172167969</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4804248097350872</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9679389035394174</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -508,13 +585,34 @@
         <v>0.9870441617067307</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.7009810269017539</v>
       </c>
       <c r="D4" t="n">
+        <v>0.4821249939228794</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.1984202670442547</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
+        <v>0.9354838709677438</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9945021362525528</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9971728378168827</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.4783596646895119</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.966573298315848</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -525,13 +623,34 @@
         <v>0.9854362437322768</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5797826902586053</v>
       </c>
       <c r="D5" t="n">
+        <v>0.4569405204233162</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.08656199145688839</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
+        <v>0.9032258064516121</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9947672778115013</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9974762822290354</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.4580164258916395</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9640820130383683</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -542,13 +661,34 @@
         <v>0.9868274138886178</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5786587501534171</v>
       </c>
       <c r="D6" t="n">
+        <v>0.5210079104301517</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.1400310125675917</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
+        <v>0.9032258064516121</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9958682181731456</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.9987548264706965</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.2823120937051792</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9538741718760513</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -559,13 +699,34 @@
         <v>0.9864722301200715</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5775465126226558</v>
       </c>
       <c r="D7" t="n">
+        <v>0.504306321230209</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.2458936684889089</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
+        <v>0.8709677419354875</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9955816851468706</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.9984148300883421</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.3408982227867237</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.956476820529933</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -576,13 +737,34 @@
         <v>0.9771003779969896</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.06436385797474525</v>
       </c>
       <c r="D8" t="n">
+        <v>0.08695502661972937</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.2415150964667461</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
+        <v>0.8709677419354875</v>
+      </c>
+      <c r="G8" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.995185475396468</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.9979469548277106</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.3934463727922193</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9600922983102562</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -593,13 +775,34 @@
         <v>0.9752647083228541</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.05806907334779704</v>
       </c>
       <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.1990315952374694</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
+        <v>0.8709677419354875</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.2769230769230769</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9938221821688548</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9963509634584204</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.6527359268372354</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.9726370191705382</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -610,13 +813,34 @@
         <v>0.9753182230985611</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.05158099855586923</v>
       </c>
       <c r="D10" t="n">
+        <v>0.0003290716849049802</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.1903645527673143</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
+        <v>0.8709677419354875</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.2615384615384616</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.9939629318159511</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.9965096290030682</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.6040928049754837</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.9712958398905062</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -627,13 +851,34 @@
         <v>0.9943879850865608</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2742923152789882</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
+        <v>0.8894476881173518</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.2656550010191824</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
+        <v>0.8709677419354875</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.2615384615384616</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9939896311834069</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.9965353093646726</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.506728251696605</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.9710078867636006</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -644,13 +889,34 @@
         <v>0.9962837117248686</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.9944724969798733</v>
       </c>
       <c r="D12" t="n">
+        <v>0.9788548120863076</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.3462302058487884</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
+        <v>0.8387096774193559</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.2461538461538461</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9956380546565073</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.9984529282936044</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.3006557725101743</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9557458204525275</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -661,13 +927,34 @@
         <v>0.995810232662944</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.9890660359218981</v>
       </c>
       <c r="D13" t="n">
+        <v>0.958626076106208</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.4094646715004119</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
+        <v>0.8064516129032278</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.2461538461538461</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9953989930665867</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.998168699772593</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.37413804795302</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.9579119267895568</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -678,13 +965,34 @@
         <v>0.9866288275135294</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.586752259017648</v>
       </c>
       <c r="D14" t="n">
+        <v>0.5131690086300654</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.3414089456541139</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
+        <v>0.7741935483870996</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.2461538461538461</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9947726047475365</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.996021278131152</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.4730736920152049</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.9666573187698657</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -695,13 +1003,34 @@
         <v>0.9856342490880072</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5860205673566089</v>
       </c>
       <c r="D15" t="n">
+        <v>0.4670372565743995</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.25355811726861</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
+        <v>0.741935483870968</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.2307692307692308</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9939813461023632</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.99510272261563</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.6349860070635606</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.9739022526346681</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -712,13 +1041,34 @@
         <v>0.988467873482236</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5852960532601483</v>
       </c>
       <c r="D16" t="n">
+        <v>0.5979719131128902</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.2052343999851028</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
+        <v>0.7096774193548399</v>
+      </c>
+      <c r="G16" t="n">
         <v>0.2307692307692308</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9962316842968993</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.9977323888800622</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.2471689513070562</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.953062076468007</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -729,13 +1079,34 @@
         <v>0.9867751665886449</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5236346045394227</v>
       </c>
       <c r="D17" t="n">
+        <v>0.5945171236907036</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.1607270861668122</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
+        <v>0.7096774193548399</v>
+      </c>
+      <c r="G17" t="n">
         <v>0.2307692307692308</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.995982922383422</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.9974466104558838</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.2813645162752761</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9552985360150279</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -746,13 +1117,34 @@
         <v>0.9859538249879723</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5234705187071165</v>
       </c>
       <c r="D18" t="n">
+        <v>0.5561242575417651</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.02668468010345873</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
+        <v>0.7096774193548399</v>
+      </c>
+      <c r="G18" t="n">
         <v>0.2307692307692308</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.9953243542867891</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.996682721566502</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.3993518297214528</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.9613194141187007</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -763,13 +1155,34 @@
         <v>0.9850945675916684</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5233071902834195</v>
       </c>
       <c r="D19" t="n">
+        <v>0.5159783552001674</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.2442050669442393</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G19" t="n">
         <v>0.2153846153846155</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.9946357069818934</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.9958837039175842</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.4918638127890506</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.9676185898792923</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -780,13 +1193,34 @@
         <v>0.9858544198824891</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5400327852829484</v>
       </c>
       <c r="D20" t="n">
+        <v>0.4769126538054654</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.2402951670397633</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G20" t="n">
         <v>0.2153846153846155</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.9950434005969891</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.996363609739512</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.4719810427311055</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.9637948380358665</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -797,13 +1231,34 @@
         <v>0.985685105223959</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5390749272057044</v>
       </c>
       <c r="D21" t="n">
+        <v>0.4685213209668389</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.2230573269855229</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G21" t="n">
         <v>0.2153846153846155</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.9949035078490781</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.9962046746427933</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.4921920362000497</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.9650278671739611</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -814,13 +1269,34 @@
         <v>0.9863376918449059</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5381240580636671</v>
       </c>
       <c r="D22" t="n">
+        <v>0.498150714237989</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.166920023182301</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
+        <v>0.6129032258064555</v>
+      </c>
+      <c r="G22" t="n">
         <v>0.2</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.9954166812195209</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.9968075486247194</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.3976005690238599</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.9602308122521267</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -831,13 +1307,34 @@
         <v>0.9843184590781249</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4511812931641361</v>
       </c>
       <c r="D23" t="n">
+        <v>0.4005695758728437</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.2701144801522594</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G23" t="n">
         <v>0.2</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.994820823746987</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.9961166186247231</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.4050553748719518</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.9656751792246812</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -848,13 +1345,34 @@
         <v>0.984392693338956</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4500417054098162</v>
       </c>
       <c r="D24" t="n">
+        <v>0.4029133234542104</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.3152016040433849</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G24" t="n">
         <v>0.1846153846153847</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.9948738321925559</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.9961825988659612</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.4666731454969064</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.9651282623410788</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -865,13 +1383,34 @@
         <v>0.9841473643561247</v>
       </c>
       <c r="C25" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4489001324552864</v>
       </c>
       <c r="D25" t="n">
+        <v>0.3904718298936434</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.4558955464589535</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
+        <v>0.6129032258064555</v>
+      </c>
+      <c r="G25" t="n">
         <v>0.1846153846153847</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.9946729850950272</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.9959524004631578</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.504271433281398</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.9669260016326096</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -882,13 +1421,34 @@
         <v>0.9899122952896006</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0.7706566902414165</v>
       </c>
       <c r="D26" t="n">
+        <v>0.7539190312873689</v>
+      </c>
+      <c r="E26" t="n">
         <v>0.333307729531285</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
+        <v>0.6129032258064555</v>
+      </c>
+      <c r="G26" t="n">
         <v>0.1846153846153847</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.9950940202586995</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.996114590095561</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.493934346505972</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.9665405811298221</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -899,13 +1459,34 @@
         <v>0.9906138658606791</v>
       </c>
       <c r="C27" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.7688278629884534</v>
       </c>
       <c r="D27" t="n">
+        <v>0.786187656232195</v>
+      </c>
+      <c r="E27" t="n">
         <v>0.2435655609722554</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G27" t="n">
         <v>0.1692307692307692</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.995680634688192</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.9968060161011242</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.4316850960443767</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.9610381658735081</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -916,13 +1497,34 @@
         <v>0.9897578234479245</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.7670225464271512</v>
       </c>
       <c r="D28" t="n">
+        <v>0.7464002524047624</v>
+      </c>
+      <c r="E28" t="n">
         <v>0.2170752063872309</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G28" t="n">
         <v>0.1692307692307692</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.9950290656500622</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.9960529401555825</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.4759716818008413</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.9669709174555586</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -933,13 +1535,34 @@
         <v>0.9873415895146681</v>
       </c>
       <c r="C29" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6580752801441139</v>
       </c>
       <c r="D29" t="n">
+        <v>0.4742790210082277</v>
+      </c>
+      <c r="E29" t="n">
         <v>0.1084437834901044</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G29" t="n">
         <v>0.1692307692307692</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.9950483330608199</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.9960823645098994</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.467607911577312</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.9667094161832184</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -950,13 +1573,34 @@
         <v>0.9874528769894533</v>
       </c>
       <c r="C30" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6561116391774811</v>
       </c>
       <c r="D30" t="n">
+        <v>0.4796845518725111</v>
+      </c>
+      <c r="E30" t="n">
         <v>0.04495510135212435</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G30" t="n">
         <v>0.1692307692307692</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.9951381108807422</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.9961939687383287</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.4694354679379368</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.9657974574043684</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -967,13 +1611,34 @@
         <v>0.987779944536664</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6541790147720429</v>
       </c>
       <c r="D31" t="n">
+        <v>0.4950692071639683</v>
+      </c>
+      <c r="E31" t="n">
         <v>0.2569507362829783</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G31" t="n">
         <v>0.1538461538461538</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.9953993145576944</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.9965054778402285</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.4420601940130754</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.9633029987871482</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -984,13 +1649,34 @@
         <v>0.9823164747191337</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3831256636519635</v>
       </c>
       <c r="D32" t="n">
+        <v>0.2661782085722706</v>
+      </c>
+      <c r="E32" t="n">
         <v>0.2315706478410685</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G32" t="n">
         <v>0.1538461538461538</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.9952194035892123</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.9963023258203161</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.4328522352647602</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.9648830981661997</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1001,13 +1687,34 @@
         <v>0.9832362912040586</v>
       </c>
       <c r="C33" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.379811041359327</v>
       </c>
       <c r="D33" t="n">
+        <v>0.3064589450522511</v>
+      </c>
+      <c r="E33" t="n">
         <v>0.2061807625340628</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G33" t="n">
         <v>0.1538461538461538</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.9959504877898057</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.9971618335049719</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.3723022077765162</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.9580503926351426</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1018,13 +1725,34 @@
         <v>0.9830088366160736</v>
       </c>
       <c r="C34" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3764662594405501</v>
       </c>
       <c r="D34" t="n">
+        <v>0.2936197551444125</v>
+      </c>
+      <c r="E34" t="n">
         <v>0.1803721512266706</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G34" t="n">
         <v>0.1538461538461538</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.9957701846767207</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.996958080577356</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.3832166305801797</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.9596354928650028</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1035,13 +1763,34 @@
         <v>0.9843912389763748</v>
       </c>
       <c r="C35" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4483929522760918</v>
       </c>
       <c r="D35" t="n">
+        <v>0.4472056667061405</v>
+      </c>
+      <c r="E35" t="n">
         <v>0.2705348590361562</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G35" t="n">
         <v>0.1538461538461538</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.9959904247857578</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.9972215152929835</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.3705152434098531</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.9575220698412108</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1052,13 +1801,34 @@
         <v>0.9846812314810857</v>
       </c>
       <c r="C36" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4475017974959454</v>
       </c>
       <c r="D36" t="n">
+        <v>0.4599552863871794</v>
+      </c>
+      <c r="E36" t="n">
         <v>0.4349513119728748</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G36" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.9962153179736744</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.9974903083212233</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.2910385964014466</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.9553663852445861</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1069,13 +1839,34 @@
         <v>0.9851162183309804</v>
       </c>
       <c r="C37" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4466088528898878</v>
       </c>
       <c r="D37" t="n">
+        <v>0.4794093222051089</v>
+      </c>
+      <c r="E37" t="n">
         <v>0.3821709698458895</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G37" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.9965555050272864</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.9978935288633971</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.2342588880723614</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.9521466689884892</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1086,13 +1877,34 @@
         <v>0.991393018555389</v>
       </c>
       <c r="C38" t="n">
-        <v>0.4671283096935754</v>
+        <v>0.5556604666921346</v>
       </c>
       <c r="D38" t="n">
+        <v>0.7224845686019766</v>
+      </c>
+      <c r="E38" t="n">
         <v>0.3415825228444795</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
+        <v>0.6774193548387082</v>
+      </c>
+      <c r="G38" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.998354141925435</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.07870096975326518</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.9391826878446033</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1103,13 +1915,34 @@
         <v>0.9877917243236148</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5554981992742091</v>
       </c>
       <c r="D39" t="n">
+        <v>0.5563397900546089</v>
+      </c>
+      <c r="E39" t="n">
         <v>0.2406521685205525</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G39" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.9954934027149097</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.9966706407825117</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.4991270461619542</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.965489893197179</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1120,13 +1953,34 @@
         <v>0.9876217748226509</v>
       </c>
       <c r="C40" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5553365782833861</v>
       </c>
       <c r="D40" t="n">
+        <v>0.5489173710093087</v>
+      </c>
+      <c r="E40" t="n">
         <v>0.1940900340808913</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G40" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.9953589958753968</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.9965215890549495</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.5066174053952723</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.9666207178331913</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1137,13 +1991,34 @@
         <v>0.9870267502304884</v>
       </c>
       <c r="C41" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5191690556526207</v>
       </c>
       <c r="D41" t="n">
+        <v>0.489496344197307</v>
+      </c>
+      <c r="E41" t="n">
         <v>0.004994594612462322</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G41" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.9958692186987508</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.9971244281140031</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.4289422565245661</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.9617994349538268</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1154,13 +2029,34 @@
         <v>0.9860957240740617</v>
       </c>
       <c r="C42" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5189665064669197</v>
       </c>
       <c r="D42" t="n">
+        <v>0.4465525826415619</v>
+      </c>
+      <c r="E42" t="n">
         <v>0.1788476025582867</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
+        <v>0.6451612903225801</v>
+      </c>
+      <c r="G42" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.9951219934079208</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.9962602976723656</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.5349905266530876</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.9685919911023991</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1171,13 +2067,34 @@
         <v>0.9863479800757787</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5187649065110128</v>
       </c>
       <c r="D43" t="n">
+        <v>0.4583495096445215</v>
+      </c>
+      <c r="E43" t="n">
         <v>0.2638817498695101</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
+        <v>0.6129032258064555</v>
+      </c>
+      <c r="G43" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.9953150310060733</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.9964929310752416</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.5101022712614719</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.9667021880574344</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1188,13 +2105,34 @@
         <v>0.987732877118478</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.590797308534841</v>
       </c>
       <c r="D44" t="n">
+        <v>0.5664361823019488</v>
+      </c>
+      <c r="E44" t="n">
         <v>0.1869401721371576</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
+        <v>0.6129032258064555</v>
+      </c>
+      <c r="G44" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.9958098187538911</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.9970774734127471</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.4545412938591608</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.9620265158749708</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1205,13 +2143,34 @@
         <v>0.9881864181755687</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5905509649962073</v>
       </c>
       <c r="D45" t="n">
+        <v>0.5876817697776895</v>
+      </c>
+      <c r="E45" t="n">
         <v>0.2673996879603596</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G45" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.9961673634858157</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.9975018209080251</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.3796449961608567</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.9586193262337169</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1222,13 +2181,34 @@
         <v>0.9890272465585122</v>
       </c>
       <c r="C46" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5903054348496281</v>
       </c>
       <c r="D46" t="n">
+        <v>0.6268443680346696</v>
+      </c>
+      <c r="E46" t="n">
         <v>0.1690781374455284</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G46" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.9968326682362012</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.9982850889800915</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.2738033829246919</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.9523708961543608</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1239,13 +2219,34 @@
         <v>0.9909213164896956</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6548301019316398</v>
       </c>
       <c r="D47" t="n">
+        <v>0.7569792848725709</v>
+      </c>
+      <c r="E47" t="n">
         <v>0.2363163490711443</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
+        <v>0.5483870967741957</v>
+      </c>
+      <c r="G47" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.9962152928447381</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.997571969778196</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.4264502145385787</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.9579696750175393</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1256,13 +2257,34 @@
         <v>0.9904442541889684</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6531911624404501</v>
       </c>
       <c r="D48" t="n">
+        <v>0.7350319270926521</v>
+      </c>
+      <c r="E48" t="n">
         <v>0.2998080533577057</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
+        <v>0.5483870967741957</v>
+      </c>
+      <c r="G48" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.9958613563441323</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.9971660760405542</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.4361074937639563</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.9611364394003525</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1273,13 +2295,34 @@
         <v>0.9912128792887085</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6515765512864212</v>
       </c>
       <c r="D49" t="n">
+        <v>0.7707207811140175</v>
+      </c>
+      <c r="E49" t="n">
         <v>0.5189598165400107</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G49" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.996496655046944</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.9979140731544557</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.3291286649421136</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.9551682272165031</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1290,13 +2333,34 @@
         <v>0.9795577609426185</v>
       </c>
       <c r="C50" t="n">
-        <v>0.2405565124923187</v>
+        <v>0.2179797793756399</v>
       </c>
       <c r="D50" t="n">
+        <v>0.2379253329618874</v>
+      </c>
+      <c r="E50" t="n">
         <v>0.3712774178393858</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G50" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.9946846773365124</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.997601163900217</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.3582333302100829</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.9607309983917958</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1307,13 +2371,34 @@
         <v>0.9801444494222538</v>
       </c>
       <c r="C51" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.2145811317510423</v>
       </c>
       <c r="D51" t="n">
+        <v>0.2637648592066592</v>
+      </c>
+      <c r="E51" t="n">
         <v>0.2432400746546668</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
+        <v>0.5806451612903238</v>
+      </c>
+      <c r="G51" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.995196885183195</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.9981926279235881</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.317139331932879</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.9559797406527168</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1324,13 +2409,34 @@
         <v>0.9784066276441539</v>
       </c>
       <c r="C52" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.2111099404182025</v>
       </c>
       <c r="D52" t="n">
+        <v>0.1820165646535209</v>
+      </c>
+      <c r="E52" t="n">
         <v>0.1791087707261851</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
+        <v>0.5483870967741957</v>
+      </c>
+      <c r="G52" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.9938631639771643</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.9966308139540744</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.527342817213182</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.9682764402574415</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1341,13 +2447,34 @@
         <v>0.9871405828036147</v>
       </c>
       <c r="C53" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5702184013069356</v>
       </c>
       <c r="D53" t="n">
+        <v>0.5428687199594108</v>
+      </c>
+      <c r="E53" t="n">
         <v>0.0275864029228233</v>
       </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
+        <v>0.5483870967741957</v>
+      </c>
+      <c r="G53" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.993412604851824</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.9960992946375503</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.5600276253743403</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.9724172516696103</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1358,13 +2485,34 @@
         <v>0.9881601820105766</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5700444041272102</v>
       </c>
       <c r="D54" t="n">
+        <v>0.590467717901734</v>
+      </c>
+      <c r="E54" t="n">
         <v>0.145915544988168</v>
       </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
+        <v>0.5161290322580641</v>
+      </c>
+      <c r="G54" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.9942356554777858</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.9970535393045784</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.4911291353516724</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.9647954030113071</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1375,13 +2523,34 @@
         <v>0.9879011361754688</v>
       </c>
       <c r="C55" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5698709075460048</v>
       </c>
       <c r="D55" t="n">
+        <v>0.5788989464901042</v>
+      </c>
+      <c r="E55" t="n">
         <v>0.2996142629395721</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
+        <v>0.5161290322580641</v>
+      </c>
+      <c r="G55" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.9940425885453623</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.9968225054880101</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.5104932049111612</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.9665581937920824</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1392,13 +2561,34 @@
         <v>0.9897248060507798</v>
       </c>
       <c r="C56" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6506747708820242</v>
       </c>
       <c r="D56" t="n">
+        <v>0.6721017379599356</v>
+      </c>
+      <c r="E56" t="n">
         <v>0.2752258901375228</v>
       </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
+        <v>0.4838709677419359</v>
+      </c>
+      <c r="G56" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.9947169183949818</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.9976033733736265</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.3560972505717873</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.9603096985690595</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1409,13 +2599,34 @@
         <v>0.9890744957073162</v>
       </c>
       <c r="C57" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6501158393872015</v>
       </c>
       <c r="D57" t="n">
+        <v>0.6426455049556629</v>
+      </c>
+      <c r="E57" t="n">
         <v>0.200639758595858</v>
       </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
+        <v>0.4516129032258078</v>
+      </c>
+      <c r="G57" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.9942228799365836</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.9970213560393755</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.4669182200412889</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.9648524551104239</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1426,13 +2637,34 @@
         <v>0.9889082572024572</v>
       </c>
       <c r="C58" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6495599367297102</v>
       </c>
       <c r="D58" t="n">
+        <v>0.6355723281365233</v>
+      </c>
+      <c r="E58" t="n">
         <v>0.1510512154546906</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
+        <v>0.4516129032258078</v>
+      </c>
+      <c r="G58" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.9941131088808379</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.9968876529027257</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.5033182562553414</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.9658462222735239</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1443,13 +2675,34 @@
         <v>0.9848945221892067</v>
       </c>
       <c r="C59" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4646521214204528</v>
       </c>
       <c r="D59" t="n">
+        <v>0.4361579907659955</v>
+      </c>
+      <c r="E59" t="n">
         <v>0.2690493955742209</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
+        <v>0.4193548387096762</v>
+      </c>
+      <c r="G59" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.9938955496083338</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.9966282643868242</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.4901319569909405</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.9678357228058145</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1460,13 +2713,34 @@
         <v>0.985937399242734</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4643104324711352</v>
       </c>
       <c r="D60" t="n">
+        <v>0.4839521322346508</v>
+      </c>
+      <c r="E60" t="n">
         <v>0.3430097150086387</v>
       </c>
-      <c r="E60" t="n">
+      <c r="F60" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G60" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.9947222734815092</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.9975871179383207</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.4353786391004341</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.9601796615295174</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1477,13 +2751,34 @@
         <v>0.9851147555301939</v>
       </c>
       <c r="C61" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4639686731875234</v>
       </c>
       <c r="D61" t="n">
+        <v>0.4454164846666762</v>
+      </c>
+      <c r="E61" t="n">
         <v>0.5149476924133661</v>
       </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
+        <v>0.3548387096774199</v>
+      </c>
+      <c r="G61" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.9940667462483728</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.9968169298634303</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.4986856164755484</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.9662146507041421</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1494,13 +2789,34 @@
         <v>0.9871505230436742</v>
       </c>
       <c r="C62" t="n">
-        <v>0.3605066671821824</v>
+        <v>0.6501859753753982</v>
       </c>
       <c r="D62" t="n">
+        <v>0.5489904012142598</v>
+      </c>
+      <c r="E62" t="n">
         <v>0.3067779291788831</v>
       </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G62" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.9933552250823668</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.996067187418036</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.5700337409100718</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.9741675116419231</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1511,13 +2827,34 @@
         <v>0.9883747944381096</v>
       </c>
       <c r="C63" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6496285745329416</v>
       </c>
       <c r="D63" t="n">
+        <v>0.6061132513400365</v>
+      </c>
+      <c r="E63" t="n">
         <v>0.2390252649926611</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G63" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.994342627755744</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.9972123085697379</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.454856946818932</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.9650207628940169</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1528,13 +2865,34 @@
         <v>0.9895448507268076</v>
       </c>
       <c r="C64" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6490742005440343</v>
       </c>
       <c r="D64" t="n">
+        <v>0.6607237015948318</v>
+      </c>
+      <c r="E64" t="n">
         <v>0.1937172887240519</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G64" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.995286753036703</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.9983070149523757</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.3578150554331625</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.9562735189784204</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1545,13 +2903,34 @@
         <v>0.9826296457361958</v>
       </c>
       <c r="C65" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4005340829130422</v>
       </c>
       <c r="D65" t="n">
+        <v>0.3528707087357045</v>
+      </c>
+      <c r="E65" t="n">
         <v>0.03828970228867895</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G65" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.9940369438912495</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.9968424970013627</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.4379823293781138</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.967792310613265</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1562,13 +2941,34 @@
         <v>0.9840412609132497</v>
       </c>
       <c r="C66" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3994136117967252</v>
       </c>
       <c r="D66" t="n">
+        <v>0.4172323887065344</v>
+      </c>
+      <c r="E66" t="n">
         <v>0.1077397968215371</v>
       </c>
-      <c r="E66" t="n">
+      <c r="F66" t="n">
+        <v>0.4193548387096762</v>
+      </c>
+      <c r="G66" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.9951604205746634</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.9981465592361854</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.3433451879440547</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.9573885046215503</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1579,13 +2979,34 @@
         <v>0.9833273750059589</v>
       </c>
       <c r="C67" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3982854331891656</v>
       </c>
       <c r="D67" t="n">
+        <v>0.3832187799351626</v>
+      </c>
+      <c r="E67" t="n">
         <v>0.251060829337223</v>
       </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
+        <v>0.4193548387096762</v>
+      </c>
+      <c r="G67" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.994595109901581</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.9974806660592865</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.410549347079741</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.9625847141759466</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1596,13 +3017,34 @@
         <v>0.9836925946078967</v>
       </c>
       <c r="C68" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3205706240938403</v>
       </c>
       <c r="D68" t="n">
+        <v>0.3574301784856681</v>
+      </c>
+      <c r="E68" t="n">
         <v>0.2398494038312665</v>
       </c>
-      <c r="E68" t="n">
+      <c r="F68" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G68" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.9949101370186373</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.9978417800738351</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.3952852113377378</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.9596490326494385</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1613,13 +3055,34 @@
         <v>0.9824784445159067</v>
       </c>
       <c r="C69" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3191213185655901</v>
       </c>
       <c r="D69" t="n">
+        <v>0.299671901356587</v>
+      </c>
+      <c r="E69" t="n">
         <v>0.2260035232727512</v>
       </c>
-      <c r="E69" t="n">
+      <c r="F69" t="n">
+        <v>0.3870967741935516</v>
+      </c>
+      <c r="G69" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.9939475745447625</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.9967126135843541</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.5609150233935125</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.9685152302080455</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1630,13 +3093,34 @@
         <v>0.9816859180769291</v>
       </c>
       <c r="C70" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3176530121481123</v>
       </c>
       <c r="D70" t="n">
+        <v>0.2614107109253322</v>
+      </c>
+      <c r="E70" t="n">
         <v>0.1572500682975594</v>
       </c>
-      <c r="E70" t="n">
+      <c r="F70" t="n">
+        <v>0.3548387096774199</v>
+      </c>
+      <c r="G70" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.9933200623009718</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.9959743576050992</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.6199503001817661</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.9742869427779088</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1647,13 +3131,34 @@
         <v>0.9836188044207614</v>
       </c>
       <c r="C71" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4467835215823885</v>
       </c>
       <c r="D71" t="n">
+        <v>0.3207191785387242</v>
+      </c>
+      <c r="E71" t="n">
         <v>0.2442393787498847</v>
       </c>
-      <c r="E71" t="n">
+      <c r="F71" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G71" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.9943487231459185</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.9971681404748164</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.4163665091399184</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.9647592257847142</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1664,13 +3169,34 @@
         <v>0.9835102671114052</v>
       </c>
       <c r="C72" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4440651573949227</v>
       </c>
       <c r="D72" t="n">
+        <v>0.3139181912875395</v>
+      </c>
+      <c r="E72" t="n">
         <v>0.4049816999836528</v>
       </c>
-      <c r="E72" t="n">
+      <c r="F72" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G72" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.9942619535947481</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.9970608032716221</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.5054531287823583</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.9655357433002423</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1681,13 +3207,34 @@
         <v>0.9836265860661397</v>
       </c>
       <c r="C73" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4413403103002275</v>
       </c>
       <c r="D73" t="n">
+        <v>0.317498417146852</v>
+      </c>
+      <c r="E73" t="n">
         <v>0.4556362771191724</v>
       </c>
-      <c r="E73" t="n">
+      <c r="F73" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G73" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.9943538685422734</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.997161968721834</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.4790655403947179</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.9646616633608113</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1698,13 +3245,34 @@
         <v>0.999498128653896</v>
       </c>
       <c r="C74" t="n">
-        <v>0.340640078685547</v>
+        <v>0.9232918407880069</v>
       </c>
       <c r="D74" t="n">
+        <v>0.8686333774777591</v>
+      </c>
+      <c r="E74" t="n">
         <v>0.3411850641581992</v>
       </c>
-      <c r="E74" t="n">
+      <c r="F74" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G74" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.9938724399467793</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.9961573971652663</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.5579617292651852</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.9735329438710333</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1715,13 +3283,34 @@
         <v>0.9997108636728107</v>
       </c>
       <c r="C75" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.91891287485493</v>
       </c>
       <c r="D75" t="n">
+        <v>0.8926261635028784</v>
+      </c>
+      <c r="E75" t="n">
         <v>0.2503820569032379</v>
       </c>
-      <c r="E75" t="n">
+      <c r="F75" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G75" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.9943745048613057</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.9967393944679769</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.5115782435314746</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.9688438384149842</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1732,13 +3321,34 @@
         <v>0.9998988608750282</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.9146256047077951</v>
       </c>
       <c r="D76" t="n">
+        <v>0.914589619057907</v>
+      </c>
+      <c r="E76" t="n">
         <v>0.2046322553457289</v>
       </c>
-      <c r="E76" t="n">
+      <c r="F76" t="n">
+        <v>0.3548387096774199</v>
+      </c>
+      <c r="G76" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.9948391914977408</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.9972778317111342</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.4066752155894716</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.9645001110870208</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1749,13 +3359,34 @@
         <v>0.9825431710178614</v>
       </c>
       <c r="C77" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4367641354802088</v>
       </c>
       <c r="D77" t="n">
+        <v>0.3765124701089489</v>
+      </c>
+      <c r="E77" t="n">
         <v>0.1347728819291013</v>
       </c>
-      <c r="E77" t="n">
+      <c r="F77" t="n">
+        <v>0.3548387096774199</v>
+      </c>
+      <c r="G77" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.9945864637892105</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.9969794267500434</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.4864555798421895</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.9667848214319522</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1766,13 +3397,34 @@
         <v>0.9825696354066686</v>
       </c>
       <c r="C78" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4351837910221035</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>0.3765589446054607</v>
       </c>
       <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.3548387096774199</v>
+      </c>
+      <c r="G78" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.9946079686490239</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.9970009638770027</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.4990037387758953</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.9665362728472044</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1783,13 +3435,34 @@
         <v>0.9829914629391346</v>
       </c>
       <c r="C79" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4335981970695192</v>
       </c>
       <c r="D79" t="n">
+        <v>0.3948959685946022</v>
+      </c>
+      <c r="E79" t="n">
         <v>0.2288761419175686</v>
       </c>
-      <c r="E79" t="n">
+      <c r="F79" t="n">
+        <v>0.3548387096774199</v>
+      </c>
+      <c r="G79" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.994943693217996</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.9973890880117569</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.443536424040789</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.9633848452105244</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1800,13 +3473,34 @@
         <v>0.985110526788161</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4291255411219423</v>
       </c>
       <c r="D80" t="n">
+        <v>0.4920496503867814</v>
+      </c>
+      <c r="E80" t="n">
         <v>0.240366264495745</v>
       </c>
-      <c r="E80" t="n">
+      <c r="F80" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G80" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.9950394677088439</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.9974973439597963</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.4183183667114636</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.9624506699879065</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1817,13 +3511,34 @@
         <v>0.9851900104851321</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.42889311231252</v>
       </c>
       <c r="D81" t="n">
+        <v>0.4950292824521041</v>
+      </c>
+      <c r="E81" t="n">
         <v>0.1913223275697164</v>
       </c>
-      <c r="E81" t="n">
+      <c r="F81" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G81" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.9950973294319542</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.9975614134152312</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.4596972479140294</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.9618671054426999</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1834,13 +3549,34 @@
         <v>0.9843961232164533</v>
       </c>
       <c r="C82" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4286598144746093</v>
       </c>
       <c r="D82" t="n">
+        <v>0.4575940123968969</v>
+      </c>
+      <c r="E82" t="n">
         <v>0.1813378669517052</v>
       </c>
-      <c r="E82" t="n">
+      <c r="F82" t="n">
+        <v>0.258064516129032</v>
+      </c>
+      <c r="G82" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0.9944612798661453</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0.9968160571318571</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.4715287686595205</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.9676953519512914</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1851,13 +3587,34 @@
         <v>0.9847588848752253</v>
       </c>
       <c r="C83" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4362149088272211</v>
       </c>
       <c r="D83" t="n">
+        <v>0.491527944102063</v>
+      </c>
+      <c r="E83" t="n">
         <v>0.3059706466229165</v>
       </c>
-      <c r="E83" t="n">
+      <c r="F83" t="n">
+        <v>0.258064516129032</v>
+      </c>
+      <c r="G83" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.994666600510919</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0.9970522196840974</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.4961603152117828</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.9657500705502127</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1868,13 +3625,34 @@
         <v>0.9854996161898454</v>
       </c>
       <c r="C84" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4361065649122033</v>
       </c>
       <c r="D84" t="n">
+        <v>0.5252252702892147</v>
+      </c>
+      <c r="E84" t="n">
         <v>0.3263306779432031</v>
       </c>
-      <c r="E84" t="n">
+      <c r="F84" t="n">
+        <v>0.258064516129032</v>
+      </c>
+      <c r="G84" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.9952499639215757</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0.997729416077502</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.3415997683456339</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.9603119476597124</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1885,13 +3663,34 @@
         <v>0.9856203106312087</v>
       </c>
       <c r="C85" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4359979072481089</v>
       </c>
       <c r="D85" t="n">
+        <v>0.5302325012518293</v>
+      </c>
+      <c r="E85" t="n">
         <v>0.4928906849039097</v>
       </c>
-      <c r="E85" t="n">
+      <c r="F85" t="n">
+        <v>0.258064516129032</v>
+      </c>
+      <c r="G85" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.9953407049145397</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.9978319931835649</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.3600564217250121</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.9594258489978714</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1902,13 +3701,34 @@
         <v>0.987630051873893</v>
       </c>
       <c r="C86" t="n">
-        <v>0.278629091183455</v>
+        <v>0.5257076711474881</v>
       </c>
       <c r="D86" t="n">
+        <v>0.6126482937010413</v>
+      </c>
+      <c r="E86" t="n">
         <v>0.3517098391132553</v>
       </c>
-      <c r="E86" t="n">
+      <c r="F86" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G86" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.9945838590796119</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0.9976450318836428</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.3647174717258458</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.9580397579119233</v>
+      </c>
+      <c r="L86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1919,13 +3739,34 @@
         <v>0.9866650695850298</v>
       </c>
       <c r="C87" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5256389744049332</v>
       </c>
       <c r="D87" t="n">
+        <v>0.5678953662289985</v>
+      </c>
+      <c r="E87" t="n">
         <v>0.2812010341538476</v>
       </c>
-      <c r="E87" t="n">
+      <c r="F87" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G87" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.9938209664587115</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0.996749637665626</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.5038792710841919</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.9650809838276905</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -1936,13 +3777,34 @@
         <v>0.9859917244742943</v>
       </c>
       <c r="C88" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5255704463959751</v>
       </c>
       <c r="D88" t="n">
+        <v>0.5366375178275835</v>
+      </c>
+      <c r="E88" t="n">
         <v>0.2264527622025843</v>
       </c>
-      <c r="E88" t="n">
+      <c r="F88" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G88" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.993289770612211</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0.9961245649114051</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.5913563343395413</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.9699815938231239</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1953,13 +3815,34 @@
         <v>0.9858376697173431</v>
       </c>
       <c r="C89" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.537847241019811</v>
       </c>
       <c r="D89" t="n">
+        <v>0.4239821285376402</v>
+      </c>
+      <c r="E89" t="n">
         <v>0.06858034507362673</v>
       </c>
-      <c r="E89" t="n">
+      <c r="F89" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G89" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.9931267730685247</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0.9959290452060005</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.5446092017417534</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.9714802479258705</v>
+      </c>
+      <c r="L89" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1970,13 +3853,34 @@
         <v>0.9871931756685116</v>
       </c>
       <c r="C90" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5371094838426973</v>
       </c>
       <c r="D90" t="n">
+        <v>0.4865873892224848</v>
+      </c>
+      <c r="E90" t="n">
         <v>0.01457088957446162</v>
       </c>
-      <c r="E90" t="n">
+      <c r="F90" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G90" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.994207859975994</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.9971848212156024</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.4097728513891348</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0.9614828871109893</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1987,13 +3891,34 @@
         <v>0.9871717338792434</v>
       </c>
       <c r="C91" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5363768768140269</v>
       </c>
       <c r="D91" t="n">
+        <v>0.4854636777616369</v>
+      </c>
+      <c r="E91" t="n">
         <v>0.2432965699612375</v>
       </c>
-      <c r="E91" t="n">
+      <c r="F91" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G91" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.9941948447949721</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0.9971643418863406</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.38649153885636</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.9615954132079207</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2004,13 +3929,34 @@
         <v>0.9894933973587041</v>
       </c>
       <c r="C92" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6207883866921341</v>
       </c>
       <c r="D92" t="n">
+        <v>0.5990978483888836</v>
+      </c>
+      <c r="E92" t="n">
         <v>0.2645247146055693</v>
       </c>
-      <c r="E92" t="n">
+      <c r="F92" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G92" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.9938641303995884</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0.996773299166626</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.4792752537025191</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.9646437228756978</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2021,13 +3967,34 @@
         <v>0.9900853997508947</v>
       </c>
       <c r="C93" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6204062124557954</v>
       </c>
       <c r="D93" t="n">
+        <v>0.6277128697112477</v>
+      </c>
+      <c r="E93" t="n">
         <v>0.2199431155930381</v>
       </c>
-      <c r="E93" t="n">
+      <c r="F93" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G93" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.9943629082773794</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0.9973499189095001</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.4312301472581591</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.9600269790545484</v>
+      </c>
+      <c r="L93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2038,13 +4005,34 @@
         <v>0.9898573471482649</v>
       </c>
       <c r="C94" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6200256447286123</v>
       </c>
       <c r="D94" t="n">
+        <v>0.6183489081621123</v>
+      </c>
+      <c r="E94" t="n">
         <v>0.1703288041101831</v>
       </c>
-      <c r="E94" t="n">
+      <c r="F94" t="n">
+        <v>0.3225806451612918</v>
+      </c>
+      <c r="G94" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.9942096392266071</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0.9971659497802496</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.4565441355295847</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.9614356136961584</v>
+      </c>
+      <c r="L94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2055,13 +4043,34 @@
         <v>0.9878557386571445</v>
       </c>
       <c r="C95" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4513167044143294</v>
       </c>
       <c r="D95" t="n">
+        <v>0.5232842784808873</v>
+      </c>
+      <c r="E95" t="n">
         <v>0.2760802453378925</v>
       </c>
-      <c r="E95" t="n">
+      <c r="F95" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G95" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.9936287710118574</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0.99648321514025</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.5099701165816628</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.9667957063588241</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2072,13 +4081,34 @@
         <v>0.9887183111622193</v>
       </c>
       <c r="C96" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4512810564696842</v>
       </c>
       <c r="D96" t="n">
+        <v>0.5637840637635735</v>
+      </c>
+      <c r="E96" t="n">
         <v>0.3884666786855087</v>
       </c>
-      <c r="E96" t="n">
+      <c r="F96" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G96" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.9943279945911894</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.9972937767233494</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.4682875810744797</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.9603266245918292</v>
+      </c>
+      <c r="L96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2089,13 +4119,34 @@
         <v>0.9875583517131562</v>
       </c>
       <c r="C97" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.4512453582694033</v>
       </c>
       <c r="D97" t="n">
+        <v>0.5106562549590865</v>
+      </c>
+      <c r="E97" t="n">
         <v>0.4537809352991061</v>
       </c>
-      <c r="E97" t="n">
+      <c r="F97" t="n">
+        <v>0.258064516129032</v>
+      </c>
+      <c r="G97" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.9934200248429703</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0.9962295470961456</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.4666626050633214</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0.9687096497014823</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2106,13 +4157,34 @@
         <v>0.9828525666923044</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1036849252461084</v>
+        <v>0.56029485709772</v>
       </c>
       <c r="D98" t="n">
+        <v>0.6920216396453176</v>
+      </c>
+      <c r="E98" t="n">
         <v>0.3363607742226571</v>
       </c>
-      <c r="E98" t="n">
+      <c r="F98" t="n">
+        <v>0.2258064516129039</v>
+      </c>
+      <c r="G98" t="n">
         <v>0.0615384615384616</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.9966606091175774</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0.9940000520166653</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0.4562957516250217</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0.9664542322535288</v>
+      </c>
+      <c r="L98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2123,13 +4195,34 @@
         <v>0.9832707470963846</v>
       </c>
       <c r="C99" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5591748333217166</v>
       </c>
       <c r="D99" t="n">
+        <v>0.7102389076858954</v>
+      </c>
+      <c r="E99" t="n">
         <v>0.2571934501628697</v>
       </c>
-      <c r="E99" t="n">
+      <c r="F99" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G99" t="n">
         <v>0.04615384615384621</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.9969689069802584</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0.9943918602276032</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.439059555797408</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.9633423732977117</v>
+      </c>
+      <c r="L99" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="100">
@@ -2140,13 +4233,34 @@
         <v>0.9851810863060856</v>
       </c>
       <c r="C100" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5580649322667803</v>
       </c>
       <c r="D100" t="n">
+        <v>0.797559851369581</v>
+      </c>
+      <c r="E100" t="n">
         <v>0.1837646401383088</v>
       </c>
-      <c r="E100" t="n">
+      <c r="F100" t="n">
+        <v>0.06451612903225978</v>
+      </c>
+      <c r="G100" t="n">
         <v>0.03076923076923083</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.9984633024678372</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.996166746521631</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.2262743642876197</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.9492734477251853</v>
+      </c>
+      <c r="L100" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="101">
@@ -2157,13 +4271,34 @@
         <v>0.9778808810652656</v>
       </c>
       <c r="C101" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.04452859441865931</v>
       </c>
       <c r="D101" t="n">
         <v>1</v>
       </c>
       <c r="E101" t="n">
         <v>1</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.03225806451612812</v>
+      </c>
+      <c r="G101" t="n">
+        <v>1</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.9998405933901486</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.9978045038706631</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.9362916290410209</v>
+      </c>
+      <c r="L101" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="102">
@@ -2174,13 +4309,34 @@
         <v>0.9740337071782869</v>
       </c>
       <c r="C102" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.02273981314889401</v>
       </c>
       <c r="D102" t="n">
+        <v>0.8282529111722068</v>
+      </c>
+      <c r="E102" t="n">
         <v>0.2227567779523529</v>
       </c>
-      <c r="E102" t="n">
+      <c r="F102" t="n">
+        <v>0.06451612903225978</v>
+      </c>
+      <c r="G102" t="n">
         <v>0.6615384615384614</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.9969240592111986</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.9944329643741209</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.3522132825430839</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.9629923664167638</v>
+      </c>
+      <c r="L102" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="103">
@@ -2191,13 +4347,34 @@
         <v>0.9723839186153446</v>
       </c>
       <c r="C103" t="n">
-        <v>0.2742923152789882</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
+        <v>0.7586767743659759</v>
+      </c>
+      <c r="E103" t="n">
         <v>0.1741398098794855</v>
       </c>
-      <c r="E103" t="n">
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
         <v>0.4615384615384615</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.9957605282449243</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0.9931058516664862</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0.6138188260274466</v>
+      </c>
+      <c r="K103" t="n">
+        <v>0.9734976021779451</v>
+      </c>
+      <c r="L103" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="104">
@@ -2208,13 +4385,34 @@
         <v>1</v>
       </c>
       <c r="C104" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.9719317582789426</v>
       </c>
       <c r="D104" t="n">
+        <v>0.4550237588267197</v>
+      </c>
+      <c r="E104" t="n">
         <v>0.1896726643824541</v>
       </c>
-      <c r="E104" t="n">
+      <c r="F104" t="n">
+        <v>0.0967741935483879</v>
+      </c>
+      <c r="G104" t="n">
         <v>0.3846153846153846</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.9960137798987808</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0.9934309547793944</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0.6223428498919439</v>
+      </c>
+      <c r="K104" t="n">
+        <v>0.9709144307873941</v>
+      </c>
+      <c r="L104" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="105">
@@ -2225,13 +4423,34 @@
         <v>0.9995044098488705</v>
       </c>
       <c r="C105" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.9613311883308102</v>
       </c>
       <c r="D105" t="n">
+        <v>0.4517539517250289</v>
+      </c>
+      <c r="E105" t="n">
         <v>0.06059514243980324</v>
       </c>
-      <c r="E105" t="n">
+      <c r="F105" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G105" t="n">
         <v>0.3076923076923077</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.9959387720189458</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0.9933726752531832</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0.568632768710604</v>
+      </c>
+      <c r="K105" t="n">
+        <v>0.9713683439790582</v>
+      </c>
+      <c r="L105" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="106">
@@ -2242,13 +4461,34 @@
         <v>0.9997999490256538</v>
       </c>
       <c r="C106" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.9511287612396013</v>
       </c>
       <c r="D106" t="n">
+        <v>0.4840606761886735</v>
+      </c>
+      <c r="E106" t="n">
         <v>0.1100517130338768</v>
       </c>
-      <c r="E106" t="n">
+      <c r="F106" t="n">
+        <v>0.1935483870967722</v>
+      </c>
+      <c r="G106" t="n">
         <v>0.2615384615384616</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.9964745252349068</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0.9940263955588495</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0.4905468607131919</v>
+      </c>
+      <c r="K106" t="n">
+        <v>0.9661813748160424</v>
+      </c>
+      <c r="L106" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="107">
@@ -2259,13 +4499,34 @@
         <v>0.9896307417847728</v>
       </c>
       <c r="C107" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.8620689391373575</v>
       </c>
       <c r="D107" t="n">
+        <v>0.6337443864798441</v>
+      </c>
+      <c r="E107" t="n">
         <v>0.06992512714493043</v>
       </c>
-      <c r="E107" t="n">
+      <c r="F107" t="n">
+        <v>0.1612903225806441</v>
+      </c>
+      <c r="G107" t="n">
         <v>0.2153846153846155</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.9971296291180909</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0.9948188903417373</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0.4091997879257664</v>
+      </c>
+      <c r="K107" t="n">
+        <v>0.9598946761274347</v>
+      </c>
+      <c r="L107" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="108">
@@ -2276,13 +4537,34 @@
         <v>0.9896886816798469</v>
       </c>
       <c r="C108" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.8582413300423124</v>
       </c>
       <c r="D108" t="n">
+        <v>0.6372520378089647</v>
+      </c>
+      <c r="E108" t="n">
         <v>0.2265731323222581</v>
       </c>
-      <c r="E108" t="n">
+      <c r="F108" t="n">
+        <v>0.1612903225806441</v>
+      </c>
+      <c r="G108" t="n">
         <v>0.2</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.9971740199981618</v>
+      </c>
+      <c r="I108" t="n">
+        <v>0.9948985503785387</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0.4466437111373774</v>
+      </c>
+      <c r="K108" t="n">
+        <v>0.9592553680439437</v>
+      </c>
+      <c r="L108" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="109">
@@ -2293,13 +4575,34 @@
         <v>0.9872801968526778</v>
       </c>
       <c r="C109" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.8544959408870758</v>
       </c>
       <c r="D109" t="n">
+        <v>0.526512813828146</v>
+      </c>
+      <c r="E109" t="n">
         <v>0.2896019127213781</v>
       </c>
-      <c r="E109" t="n">
+      <c r="F109" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G109" t="n">
         <v>0.1846153846153847</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.9952586711341401</v>
+      </c>
+      <c r="I109" t="n">
+        <v>0.9926917570029543</v>
+      </c>
+      <c r="J109" t="n">
+        <v>0.5321018246348093</v>
+      </c>
+      <c r="K109" t="n">
+        <v>0.9767310302830582</v>
+      </c>
+      <c r="L109" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="110">
@@ -2310,13 +4613,34 @@
         <v>0.9896151174094895</v>
       </c>
       <c r="C110" t="n">
-        <v>0.6869021473603801</v>
+        <v>0.5609620488123042</v>
       </c>
       <c r="D110" t="n">
+        <v>0.5725633376091968</v>
+      </c>
+      <c r="E110" t="n">
         <v>0.2641593699030962</v>
       </c>
-      <c r="E110" t="n">
+      <c r="F110" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G110" t="n">
         <v>0.1538461538461538</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.999902171747469</v>
+      </c>
+      <c r="I110" t="n">
+        <v>0.9984096947783355</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0.4943928131909315</v>
+      </c>
+      <c r="K110" t="n">
+        <v>0.9747526090468045</v>
+      </c>
+      <c r="L110" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="111">
@@ -2327,13 +4651,34 @@
         <v>0.9898373272016392</v>
       </c>
       <c r="C111" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.559071232293224</v>
       </c>
       <c r="D111" t="n">
+        <v>0.5819382967194469</v>
+      </c>
+      <c r="E111" t="n">
         <v>0.2804731875458239</v>
       </c>
-      <c r="E111" t="n">
+      <c r="F111" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G111" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H111" t="n">
+        <v>1</v>
+      </c>
+      <c r="I111" t="n">
+        <v>0.9986336067838363</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.5855552089591999</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0.9726478689356843</v>
+      </c>
+      <c r="L111" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="112">
@@ -2344,13 +4689,34 @@
         <v>0.9883049934135102</v>
       </c>
       <c r="C112" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.5571982010124786</v>
       </c>
       <c r="D112" t="n">
+        <v>0.5100611333081445</v>
+      </c>
+      <c r="E112" t="n">
         <v>0.2140293398894549</v>
       </c>
-      <c r="E112" t="n">
+      <c r="F112" t="n">
+        <v>0.1612903225806441</v>
+      </c>
+      <c r="G112" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.9987069057372708</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0.9972307582780363</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0.6801679785195373</v>
+      </c>
+      <c r="K112" t="n">
+        <v>0.9834387148438586</v>
+      </c>
+      <c r="L112" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="113">
@@ -2361,13 +4727,34 @@
         <v>0.9894961333120041</v>
       </c>
       <c r="C113" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6671395198862945</v>
       </c>
       <c r="D113" t="n">
+        <v>0.715469545926922</v>
+      </c>
+      <c r="E113" t="n">
         <v>0.07571153649013401</v>
       </c>
-      <c r="E113" t="n">
+      <c r="F113" t="n">
+        <v>0.1935483870967722</v>
+      </c>
+      <c r="G113" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.9988594761072263</v>
+      </c>
+      <c r="I113" t="n">
+        <v>0.9975102184825454</v>
+      </c>
+      <c r="J113" t="n">
+        <v>0.681290936005489</v>
+      </c>
+      <c r="K113" t="n">
+        <v>0.9809057856832755</v>
+      </c>
+      <c r="L113" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="114">
@@ -2378,13 +4765,34 @@
         <v>0.9895562157489296</v>
       </c>
       <c r="C114" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6664640958530516</v>
       </c>
       <c r="D114" t="n">
+        <v>0.7184692526016335</v>
+      </c>
+      <c r="E114" t="n">
         <v>0.1534945131624844</v>
       </c>
-      <c r="E114" t="n">
+      <c r="F114" t="n">
+        <v>0.1935483870967722</v>
+      </c>
+      <c r="G114" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0.998853419161259</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0.9976008059658086</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0.7097890436050871</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0.979874732390936</v>
+      </c>
+      <c r="L114" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="115">
@@ -2395,13 +4803,34 @@
         <v>0.9892051087495881</v>
       </c>
       <c r="C115" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.6657928511197898</v>
       </c>
       <c r="D115" t="n">
+        <v>0.7024070999775393</v>
+      </c>
+      <c r="E115" t="n">
         <v>0.2038594155648589</v>
       </c>
-      <c r="E115" t="n">
+      <c r="F115" t="n">
+        <v>0.2258064516129039</v>
+      </c>
+      <c r="G115" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0.9985228443052774</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0.9973092113345309</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0.7918698206865462</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0.9818776518647443</v>
+      </c>
+      <c r="L115" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="116">
@@ -2412,13 +4841,34 @@
         <v>0.9850576326392908</v>
       </c>
       <c r="C116" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3853663567467568</v>
       </c>
       <c r="D116" t="n">
+        <v>0.5797702477465246</v>
+      </c>
+      <c r="E116" t="n">
         <v>0.1078235697140766</v>
       </c>
-      <c r="E116" t="n">
+      <c r="F116" t="n">
+        <v>0.2258064516129039</v>
+      </c>
+      <c r="G116" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0.9988606903305294</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0.9977938574840879</v>
+      </c>
+      <c r="J116" t="n">
+        <v>0.5933676549433829</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0.9777341744656977</v>
+      </c>
+      <c r="L116" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="117">
@@ -2429,13 +4879,34 @@
         <v>0.9854063261166083</v>
       </c>
       <c r="C117" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3852363498985255</v>
       </c>
       <c r="D117" t="n">
+        <v>0.5930508143198971</v>
+      </c>
+      <c r="E117" t="n">
         <v>0.2444482692276145</v>
       </c>
-      <c r="E117" t="n">
+      <c r="F117" t="n">
+        <v>0.1935483870967722</v>
+      </c>
+      <c r="G117" t="n">
         <v>0.1384615384615385</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.9990359184503917</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0.9980855265928924</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0.5369842896455852</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0.9751247411652975</v>
+      </c>
+      <c r="L117" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="118">
@@ -2446,13 +4917,34 @@
         <v>0.9858683419125577</v>
       </c>
       <c r="C118" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3851058916715364</v>
       </c>
       <c r="D118" t="n">
+        <v>0.6116437914262436</v>
+      </c>
+      <c r="E118" t="n">
         <v>0.0825087633232974</v>
       </c>
-      <c r="E118" t="n">
+      <c r="F118" t="n">
+        <v>0.1935483870967722</v>
+      </c>
+      <c r="G118" t="n">
         <v>0.1230769230769231</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0.9993043748508661</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0.998482817439391</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0.5733056891296506</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0.9716828912948247</v>
+      </c>
+      <c r="L118" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="119">
@@ -2463,13 +4955,34 @@
         <v>0.9851557359317356</v>
       </c>
       <c r="C119" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3597191424812062</v>
       </c>
       <c r="D119" t="n">
+        <v>0.4765668686239572</v>
+      </c>
+      <c r="E119" t="n">
         <v>0.1926279730688892</v>
       </c>
-      <c r="E119" t="n">
+      <c r="F119" t="n">
+        <v>0.1612903225806441</v>
+      </c>
+      <c r="G119" t="n">
         <v>0.1076923076923077</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0.9980196126857103</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0.9970653603225961</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0.7869501147721993</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0.9826292188753706</v>
+      </c>
+      <c r="L119" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="120">
@@ -2480,13 +4993,34 @@
         <v>0.984919735469224</v>
       </c>
       <c r="C120" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3591980326968569</v>
       </c>
       <c r="D120" t="n">
+        <v>0.462786105275483</v>
+      </c>
+      <c r="E120" t="n">
         <v>0.3775200261392984</v>
       </c>
-      <c r="E120" t="n">
+      <c r="F120" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G120" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0.9977443900911172</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0.9968226702045127</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0.7086646182002438</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0.9842700119624287</v>
+      </c>
+      <c r="L120" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -2497,13 +5031,34 @@
         <v>0.985312911327368</v>
       </c>
       <c r="C121" t="n">
-        <v>0.2742923152789882</v>
+        <v>0.3586724710518523</v>
       </c>
       <c r="D121" t="n">
+        <v>0.4782006837676019</v>
+      </c>
+      <c r="E121" t="n">
         <v>0.4342934994517286</v>
       </c>
-      <c r="E121" t="n">
+      <c r="F121" t="n">
+        <v>0.0967741935483879</v>
+      </c>
+      <c r="G121" t="n">
         <v>0.09230769230769231</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0.9979718306455284</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0.9971636194093563</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0.6505070675988471</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0.981289234280188</v>
+      </c>
+      <c r="L121" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2517,10 +5072,31 @@
         <v>0</v>
       </c>
       <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
         <v>0.4079363369724504</v>
       </c>
-      <c r="E122" t="n">
+      <c r="F122" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G122" t="n">
         <v>0.07692307692307693</v>
+      </c>
+      <c r="H122" t="n">
+        <v>0.9930220056332958</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0.996536446132341</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0.6833060359507753</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0.9807111507994541</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="123">
@@ -2534,10 +5110,31 @@
         <v>0</v>
       </c>
       <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
         <v>0.2447512174724679</v>
       </c>
-      <c r="E123" t="n">
+      <c r="F123" t="n">
+        <v>0.1290322580645196</v>
+      </c>
+      <c r="G123" t="n">
         <v>0.04615384615384621</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0.9927233403986165</v>
+      </c>
+      <c r="I123" t="n">
+        <v>0.9961695643559563</v>
+      </c>
+      <c r="J123" t="n">
+        <v>0.7548506731960245</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0.9834275684871278</v>
+      </c>
+      <c r="L123" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="124">
@@ -2551,10 +5148,31 @@
         <v>0</v>
       </c>
       <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="n">
         <v>0.2219290711988536</v>
       </c>
-      <c r="E124" t="n">
+      <c r="F124" t="n">
+        <v>0.1612903225806441</v>
+      </c>
+      <c r="G124" t="n">
         <v>0.03076923076923083</v>
+      </c>
+      <c r="H124" t="n">
+        <v>0.9911066272179969</v>
+      </c>
+      <c r="I124" t="n">
+        <v>0.9942655179662935</v>
+      </c>
+      <c r="J124" t="n">
+        <v>0.9618970566512602</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0.9983337449731385</v>
+      </c>
+      <c r="L124" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="125">
@@ -2568,10 +5186,31 @@
         <v>0</v>
       </c>
       <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
         <v>0.0025840470772025</v>
       </c>
-      <c r="E125" t="n">
-        <v>0</v>
+      <c r="F125" t="n">
+        <v>0.1935483870967722</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" t="n">
+        <v>0.9944956527615186</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0.9982007542252914</v>
+      </c>
+      <c r="J125" t="n">
+        <v>0.5362716851339961</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0.9669481793166751</v>
+      </c>
+      <c r="L125" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="126">
@@ -2585,10 +5224,31 @@
         <v>0</v>
       </c>
       <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
         <v>0.02717293657661712</v>
       </c>
-      <c r="E126" t="n">
-        <v>0</v>
+      <c r="F126" t="n">
+        <v>0.258064516129032</v>
+      </c>
+      <c r="G126" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" t="n">
+        <v>0.992650667152492</v>
+      </c>
+      <c r="I126" t="n">
+        <v>0.9960309948663526</v>
+      </c>
+      <c r="J126" t="n">
+        <v>0.8373213481418396</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0.983965977254543</v>
+      </c>
+      <c r="L126" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="127">
@@ -2602,10 +5262,31 @@
         <v>0</v>
       </c>
       <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
         <v>0.257309737740098</v>
       </c>
-      <c r="E127" t="n">
-        <v>0</v>
+      <c r="F127" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" t="n">
+        <v>0.9909123498035324</v>
+      </c>
+      <c r="I127" t="n">
+        <v>0.9939859258176579</v>
+      </c>
+      <c r="J127" t="n">
+        <v>1</v>
+      </c>
+      <c r="K127" t="n">
+        <v>1</v>
+      </c>
+      <c r="L127" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="128">
@@ -2619,10 +5300,31 @@
         <v>0</v>
       </c>
       <c r="D128" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" t="n">
         <v>0.2716846568714628</v>
       </c>
-      <c r="E128" t="n">
-        <v>0</v>
+      <c r="F128" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" t="n">
+        <v>0.9958090459464459</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0.9996806237504183</v>
+      </c>
+      <c r="J128" t="n">
+        <v>0.3707296219929684</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0.9546659025765803</v>
+      </c>
+      <c r="L128" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="129">
@@ -2636,10 +5338,31 @@
         <v>0</v>
       </c>
       <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
         <v>0.1928000425180111</v>
       </c>
-      <c r="E129" t="n">
-        <v>0</v>
+      <c r="F129" t="n">
+        <v>0.2903225806451637</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" t="n">
+        <v>0.9941645975668771</v>
+      </c>
+      <c r="I129" t="n">
+        <v>0.9977455742032486</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0.4356150255383813</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0.9698313082519218</v>
+      </c>
+      <c r="L129" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="130">
@@ -2653,10 +5376,31 @@
         <v>0</v>
       </c>
       <c r="D130" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" t="n">
         <v>0.2186608676624533</v>
       </c>
-      <c r="E130" t="n">
-        <v>0</v>
+      <c r="F130" t="n">
+        <v>0.2258064516129039</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" t="n">
+        <v>0.993815420540254</v>
+      </c>
+      <c r="I130" t="n">
+        <v>0.9973216654516615</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0.5617259035703712</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0.9730170184310524</v>
+      </c>
+      <c r="L130" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="131">
@@ -2670,10 +5414,31 @@
         <v>0</v>
       </c>
       <c r="D131" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" t="n">
         <v>0.2190729911806084</v>
       </c>
-      <c r="E131" t="n">
-        <v>0</v>
+      <c r="F131" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" t="n">
+        <v>0.9936592828625714</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0.9971231783217135</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0.5863861258720136</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0.9744176722955573</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="132">
@@ -2687,10 +5452,31 @@
         <v>0</v>
       </c>
       <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
         <v>0.3842462459056604</v>
       </c>
-      <c r="E132" t="n">
-        <v>0</v>
+      <c r="F132" t="n">
+        <v>0</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" t="n">
+        <v>0.9949261735856471</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0.9985848455143033</v>
+      </c>
+      <c r="J132" t="n">
+        <v>0.4252858022654106</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0.9626555518560601</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="133">
@@ -2708,6 +5494,27 @@
       </c>
       <c r="E133" t="n">
         <v>0</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0.9951256303983574</v>
+      </c>
+      <c r="I133" t="n">
+        <v>0.9988016277841398</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.9607671626147806</v>
+      </c>
+      <c r="L133" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>